<commit_message>
250410_dsss unquant and 3bit soft simulating
</commit_message>
<xml_diff>
--- a/Mat_sim_results/250409软判决评估/最终仿真数据.xlsx
+++ b/Mat_sim_results/250409软判决评估/最终仿真数据.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic_D\MyProjects\Github_Desktop_repos\Convolutional_Code_Matlab_Simulation\Mat_sim_results\250409软判决评估\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myProjects\Convolutional-Code_Spread-Spectrum-Communication_Matlab-Verilog\Mat_sim_results\250409软判决评估\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B7826A-3E7D-4C2A-A00E-CDCE0D6BE648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC6810F-2C44-49E3-B643-78775587EF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="各曲线结果" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>SNR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,6 +49,30 @@
   <si>
     <t>ASK</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ber_num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ber_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv+dsss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>soft-3bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -117,10 +141,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -398,276 +422,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915B004B-2A02-462E-8F0E-4CE482DBA853}">
-  <dimension ref="A2:U21"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-8</v>
       </c>
       <c r="B3">
         <v>0.42211284492187501</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-8</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.39371616484374999</v>
       </c>
-      <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-7</v>
       </c>
       <c r="B4">
         <v>0.396490619140625</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-7</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.35828155625000002</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-6</v>
       </c>
       <c r="B5">
         <v>0.36241556484374998</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-6</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.31192376171875003</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-5</v>
       </c>
       <c r="B6">
         <v>0.31802633398437502</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-5</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.253969163671875</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-4</v>
       </c>
       <c r="B7">
         <v>0.26270231328124999</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-4</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.1872029015625</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-3</v>
       </c>
       <c r="B8">
         <v>0.19864080742187501</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>-3</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.119530429296875</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-2</v>
       </c>
       <c r="B9">
         <v>0.13272199570312501</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>-2</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>6.2841107031249996E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-1</v>
       </c>
       <c r="B10">
         <v>7.5208687499999996E-2</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>-1</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2.5880946875000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
       <c r="B11">
         <v>3.4830464453125001E-2</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>8.0798160156249996E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
         <v>1.2815395703124999E-2</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1.90035625E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
         <v>3.70647890625E-3</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>3.5824843750000002E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14">
         <v>8.5755351562499999E-4</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>6.4742187499999994E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15">
         <v>1.7597421875000001E-4</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>4</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>1.4084375E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>3.8947656249999998E-5</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>5</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>3.5437500000000002E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>1.078515625E-5</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>6</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>8.9335937500000001E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
       <c r="B18" s="2">
         <v>3.1460937499999998E-6</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>7</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>1.5937500000000001E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
       <c r="B19" s="2">
         <v>7.5820312500000001E-7</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>8</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>2.1484374999999999E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -675,7 +743,7 @@
         <v>1.3359374999999999E-7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
@@ -684,6 +752,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -692,27 +764,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F959FB89-A7BB-48DF-BB1C-7EB03A9E8811}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:AK27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,158 +794,590 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-8</v>
       </c>
       <c r="B3">
         <v>0.286714527581443</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.28671928554687498</v>
+      </c>
+      <c r="D3">
+        <v>996218913</v>
+      </c>
+      <c r="F3">
+        <v>-8</v>
+      </c>
+      <c r="H3">
+        <v>0.38914801289062501</v>
+      </c>
+      <c r="I3">
+        <v>734001371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-7</v>
       </c>
       <c r="B4">
         <v>0.26378950525626599</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0.2637965203125</v>
+      </c>
+      <c r="D4">
+        <v>962661529</v>
+      </c>
+      <c r="F4">
+        <v>-7</v>
+      </c>
+      <c r="H4">
+        <v>0.37603965976562498</v>
+      </c>
+      <c r="I4">
+        <v>675319092</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-6</v>
       </c>
       <c r="B5">
         <v>0.23922871076767199</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0.239240996484375</v>
+      </c>
+      <c r="D5">
+        <v>925486407</v>
+      </c>
+      <c r="F5">
+        <v>-6</v>
+      </c>
+      <c r="H5">
+        <v>0.36151812773437503</v>
+      </c>
+      <c r="I5">
+        <v>612456951</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-5</v>
       </c>
       <c r="B6">
         <v>0.21322801835762001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0.21323373046874999</v>
+      </c>
+      <c r="D6">
+        <v>884345292</v>
+      </c>
+      <c r="F6">
+        <v>-5</v>
+      </c>
+      <c r="H6">
+        <v>0.3454473796875</v>
+      </c>
+      <c r="I6">
+        <v>545878350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-4</v>
       </c>
       <c r="B7">
         <v>0.18611381748338901</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0.18610776679687499</v>
+      </c>
+      <c r="D7">
+        <v>839019382</v>
+      </c>
+      <c r="F7">
+        <v>-4</v>
+      </c>
+      <c r="H7">
+        <v>0.32774194609375001</v>
+      </c>
+      <c r="I7">
+        <v>476435883</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-3</v>
       </c>
       <c r="B8">
         <v>0.15836831880959801</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.15836266484375</v>
+      </c>
+      <c r="D8">
+        <v>789339543</v>
+      </c>
+      <c r="F8">
+        <v>-3</v>
+      </c>
+      <c r="H8">
+        <v>0.30833575898437499</v>
+      </c>
+      <c r="I8">
+        <v>405408422</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-2</v>
       </c>
       <c r="B9">
         <v>0.13064448852282901</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.130642015625</v>
+      </c>
+      <c r="D9">
+        <v>735176571</v>
+      </c>
+      <c r="F9">
+        <v>-2</v>
+      </c>
+      <c r="H9">
+        <v>0.28717834804687498</v>
+      </c>
+      <c r="I9">
+        <v>334443560</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-1</v>
       </c>
       <c r="B10">
         <v>0.103759095953406</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.1037518671875</v>
+      </c>
+      <c r="D10">
+        <v>676541319</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>0.26427395273437498</v>
+      </c>
+      <c r="I10">
+        <v>265604780</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
       <c r="B11">
         <v>7.8649603525142595E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>7.8648814843749998E-2</v>
+      </c>
+      <c r="D11">
+        <v>613786870</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.23976049609375</v>
+      </c>
+      <c r="I11">
+        <v>201340966</v>
+      </c>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
         <v>5.6281951976541497E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>5.6284738671875001E-2</v>
+      </c>
+      <c r="D12">
+        <v>547253782</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.21377100859375001</v>
+      </c>
+      <c r="I12">
+        <v>144088931</v>
+      </c>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
         <v>3.7506128358926E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>3.7503370312499999E-2</v>
+      </c>
+      <c r="D13">
+        <v>477940890</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>0.18669566015625</v>
+      </c>
+      <c r="I13">
+        <v>96008628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14">
         <v>2.28784075610853E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2.2877808984375001E-2</v>
+      </c>
+      <c r="D14">
+        <v>406902544</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0.15894630625</v>
+      </c>
+      <c r="I14">
+        <v>58567191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15">
         <v>1.2500818040737599E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1.2499623046875E-2</v>
+      </c>
+      <c r="D15">
+        <v>335883068</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0.13120432343749999</v>
+      </c>
+      <c r="I15">
+        <v>31999035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16">
         <v>5.9538671477786598E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>5.9545031249999998E-3</v>
+      </c>
+      <c r="D16">
+        <v>266986016</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>0.1042914125</v>
+      </c>
+      <c r="I16">
+        <v>15243528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17">
         <v>2.3882907809328101E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2.3878851562500001E-3</v>
+      </c>
+      <c r="D17">
+        <v>202616177</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>7.9146944140624995E-2</v>
+      </c>
+      <c r="I17">
+        <v>6112986</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
       <c r="B18">
         <v>7.7267481537844401E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>7.7252265624999997E-4</v>
+      </c>
+      <c r="D18">
+        <v>145168369</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>5.6706394140624998E-2</v>
+      </c>
+      <c r="I18">
+        <v>1977658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
       <c r="B19">
         <v>1.9090777407599301E-4</v>
+      </c>
+      <c r="C19">
+        <v>1.9085507812499999E-4</v>
+      </c>
+      <c r="D19">
+        <v>96890552</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>3.7847871875000001E-2</v>
+      </c>
+      <c r="I19">
+        <v>488589</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.3333984374999998E-5</v>
+      </c>
+      <c r="D20">
+        <v>59234453</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>2.3138458203125E-2</v>
+      </c>
+      <c r="I20">
+        <v>85335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.9230468750000003E-6</v>
+      </c>
+      <c r="D21">
+        <v>32451661</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>1.2676430078125E-2</v>
+      </c>
+      <c r="I21">
+        <v>10043</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2.5781250000000002E-7</v>
+      </c>
+      <c r="D22">
+        <v>15501955</v>
+      </c>
+      <c r="F22">
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>6.0554511718750002E-3</v>
+      </c>
+      <c r="I22">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2">
+        <v>7.0312499999999997E-9</v>
+      </c>
+      <c r="D23">
+        <v>6236568</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>2.436159375E-3</v>
+      </c>
+      <c r="I23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.9062499999999998E-10</v>
+      </c>
+      <c r="D24">
+        <v>2029765</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="H24">
+        <v>7.9287695312500002E-4</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>504401</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="H25">
+        <v>1.9703164062500001E-4</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>89513</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3.4966015625000002E-5</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>10613</v>
+      </c>
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="H27" s="2">
+        <v>4.1457031250000002E-6</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
250411_dsss 3bit soft simresult stored
</commit_message>
<xml_diff>
--- a/Mat_sim_results/250409软判决评估/最终仿真数据.xlsx
+++ b/Mat_sim_results/250409软判决评估/最终仿真数据.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myProjects\Convolutional-Code_Spread-Spectrum-Communication_Matlab-Verilog\Mat_sim_results\250409软判决评估\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC6810F-2C44-49E3-B643-78775587EF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805FDC33-D636-4CA7-86BF-6C92B9C3B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>SNR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,12 +74,52 @@
     <t>hard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>L=256, (2,1,3), g=[5 7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L=8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, (2,1,3), g=[5 7], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tb_lenth=8,!=5v</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +148,33 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,7 +191,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -145,6 +205,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -422,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915B004B-2A02-462E-8F0E-4CE482DBA853}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -434,327 +503,499 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-8</v>
-      </c>
-      <c r="B3">
-        <v>0.42211284492187501</v>
-      </c>
-      <c r="E3">
-        <v>-8</v>
-      </c>
-      <c r="F3">
-        <v>0.39371616484374999</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B4">
-        <v>0.396490619140625</v>
+        <v>0.42211284492187501</v>
       </c>
       <c r="E4">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F4">
-        <v>0.35828155625000002</v>
-      </c>
+        <v>0.39371616484374999</v>
+      </c>
+      <c r="M4">
+        <v>-8</v>
+      </c>
+      <c r="N4">
+        <v>1.5897518749999999E-2</v>
+      </c>
+      <c r="O4">
+        <v>40697648</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B5">
-        <v>0.36241556484374998</v>
+        <v>0.396490619140625</v>
       </c>
       <c r="E5">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="F5">
-        <v>0.31192376171875003</v>
+        <v>0.35828155625000002</v>
+      </c>
+      <c r="M5">
+        <v>-7</v>
+      </c>
+      <c r="N5">
+        <v>4.5349328124999998E-3</v>
+      </c>
+      <c r="O5">
+        <v>11609428</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="B6">
-        <v>0.31802633398437502</v>
+        <v>0.36241556484374998</v>
       </c>
       <c r="E6">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="F6">
-        <v>0.253969163671875</v>
+        <v>0.31192376171875003</v>
+      </c>
+      <c r="M6">
+        <v>-6</v>
+      </c>
+      <c r="N6">
+        <v>9.9803984375000003E-4</v>
+      </c>
+      <c r="O6">
+        <v>2554982</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="B7">
-        <v>0.26270231328124999</v>
+        <v>0.31802633398437502</v>
       </c>
       <c r="E7">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="F7">
-        <v>0.1872029015625</v>
+        <v>0.253969163671875</v>
+      </c>
+      <c r="M7">
+        <v>-5</v>
+      </c>
+      <c r="N7">
+        <v>1.8676171875E-4</v>
+      </c>
+      <c r="O7">
+        <v>478110</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="B8">
-        <v>0.19864080742187501</v>
+        <v>0.26270231328124999</v>
       </c>
       <c r="E8">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="F8">
-        <v>0.119530429296875</v>
+        <v>0.1872029015625</v>
+      </c>
+      <c r="M8">
+        <v>-4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3.7101562499999998E-5</v>
+      </c>
+      <c r="O8">
+        <v>94980</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B9">
-        <v>0.13272199570312501</v>
+        <v>0.19864080742187501</v>
       </c>
       <c r="E9">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F9">
-        <v>6.2841107031249996E-2</v>
+        <v>0.119530429296875</v>
+      </c>
+      <c r="M9">
+        <v>-3</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9.3203125000000004E-6</v>
+      </c>
+      <c r="O9">
+        <v>23860</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B10">
-        <v>7.5208687499999996E-2</v>
+        <v>0.13272199570312501</v>
       </c>
       <c r="E10">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F10">
-        <v>2.5880946875000001E-2</v>
+        <v>6.2841107031249996E-2</v>
+      </c>
+      <c r="M10">
+        <v>-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2.466015625E-6</v>
+      </c>
+      <c r="O10">
+        <v>6313</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B11">
-        <v>3.4830464453125001E-2</v>
+        <v>7.5208687499999996E-2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11">
-        <v>8.0798160156249996E-3</v>
+        <v>2.5880946875000001E-2</v>
+      </c>
+      <c r="M11">
+        <v>-1</v>
+      </c>
+      <c r="N11" s="2">
+        <v>5.4453125E-7</v>
+      </c>
+      <c r="O11">
+        <v>1394</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>1.2815395703124999E-2</v>
+        <v>3.4830464453125001E-2</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1.90035625E-3</v>
+        <v>8.0798160156249996E-3</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>3.70647890625E-3</v>
+        <v>1.2815395703124999E-2</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>3.5824843750000002E-4</v>
+        <v>1.90035625E-3</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>8.5755351562499999E-4</v>
+        <v>3.70647890625E-3</v>
       </c>
       <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
-        <v>6.4742187499999994E-5</v>
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>3.5824843750000002E-4</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>1.7597421875000001E-4</v>
+        <v>8.5755351562499999E-4</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="2">
-        <v>1.4084375E-5</v>
+        <v>6.4742187499999994E-5</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1.7597421875000001E-4</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.4084375E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>5</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>3.8947656249999998E-5</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>5</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>3.5437500000000002E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>6</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>1.078515625E-5</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>6</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>8.9335937500000001E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>7</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>3.1460937499999998E-6</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>7</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>1.5937500000000001E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>8</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="2">
         <v>7.5820312500000001E-7</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>8</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>2.1484374999999999E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>9</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B21" s="2">
         <v>1.3359374999999999E-7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>10</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="2">
         <v>1.4062499999999999E-8</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="I25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="I25:O25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>